<commit_message>
rangement des données d'études + ajout des pdf trouvé sur le site capacity4Dev
</commit_message>
<xml_diff>
--- a/data/xls/to_do/Guinea Bissau-Social model V1 - Frutas e Legumes.xlsx
+++ b/data/xls/to_do/Guinea Bissau-Social model V1 - Frutas e Legumes.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">Value chain:</t>
   </si>
   <si>
-    <t xml:space="preserve">Manga/ Lima</t>
+    <t xml:space="preserve">mango</t>
   </si>
   <si>
     <t xml:space="preserve">Country :</t>
@@ -502,16 +502,8 @@
     <t xml:space="preserve">4.3 Utilisation and nutritional adequacy </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">4.3.1 Is the nutritional quality of available food improving?  
+    <t xml:space="preserve">4.3.1 Is the nutritional quality of available food improving?  
 </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Os trabalhadores assalariados  gozam de uma estabilidade económica que lhes garante uma maior qualidade nutricional. </t>
@@ -4686,7 +4678,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="172">
+  <dxfs count="144">
     <dxf>
       <fill>
         <patternFill>
@@ -4964,202 +4956,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF31859C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF77933C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF785B97"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF93CDDD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF948A54"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB1A0C7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB3A2C7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFBFBFBF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC3D69B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC4BD97"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD99694"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDBEEF4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDDD9C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE46C0A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE6B9B8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE6E0EC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEBF1DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF2DCDB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFAC090"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFDEADA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC0C0C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5967,10 +5763,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.247977795400476"/>
-          <c:y val="0.192106790481718"/>
-          <c:w val="0.509833465503569"/>
-          <c:h val="0.509825055965509"/>
+          <c:x val="0.247920133111481"/>
+          <c:y val="0.19212271973466"/>
+          <c:w val="0.50978527850408"/>
+          <c:h val="0.509784411276949"/>
         </c:manualLayout>
       </c:layout>
       <c:radarChart>
@@ -6208,13 +6004,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="71727307"/>
-        <c:axId val="11154950"/>
+        <c:axId val="74417547"/>
+        <c:axId val="34051491"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="71727307"/>
+        <c:axId val="74417547"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -6251,7 +6047,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11154950"/>
+        <c:crossAx val="34051491"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6259,7 +6055,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11154950"/>
+        <c:axId val="34051491"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -6303,7 +6099,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71727307"/>
+        <c:crossAx val="74417547"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6366,9 +6162,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>300240</xdr:colOff>
+      <xdr:colOff>299880</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1240560</xdr:rowOff>
+      <xdr:rowOff>1240200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6377,7 +6173,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6564240" y="823320"/>
-        <a:ext cx="4539240" cy="4341600"/>
+        <a:ext cx="4543200" cy="4341240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6403,15 +6199,15 @@
       <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="0" width="10.85"/>
   </cols>
   <sheetData>
@@ -6851,7 +6647,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{AB26A027-B310-40B4-9468-C369DA867B24}">
+          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{B6AF56BD-DC6A-41D2-B280-7C5B153521F0}">
             <xm:f>Register!$L$6</xm:f>
             <x14:dxf>
               <fill>
@@ -6861,7 +6657,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{346A705D-7EA0-468C-BBB0-60ECE9E3BC68}">
+          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{13D04B78-B3AF-47DF-99F6-85C0FBFCCCCA}">
             <xm:f>Register!$L$5</xm:f>
             <x14:dxf>
               <fill>
@@ -6871,7 +6667,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{A076A75C-D6E6-4049-8713-1F1BFEC3B082}">
+          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{E1B0F8D4-4FD7-44CC-A78A-42275660C318}">
             <xm:f>Register!$L$4</xm:f>
             <x14:dxf>
               <fill>
@@ -6881,7 +6677,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{B9D10078-4BC9-4DD1-91A0-90DAA0BC4FAE}">
+          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{2960A1A5-A343-498C-9F44-E4DCADC42AC0}">
             <xm:f>Register!$L$3</xm:f>
             <x14:dxf>
               <fill>
@@ -6912,7 +6708,7 @@
       <selection pane="bottomLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="62" width="10.29"/>
@@ -6923,16 +6719,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="62" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="56" width="14.15"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="10" min="10" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="13" style="0" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="69" customFormat="true" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="63" t="str">
         <f aca="false">Profile!F1</f>
-        <v>Manga/ Lima</v>
+        <v>mango</v>
       </c>
       <c r="B1" s="63"/>
       <c r="C1" s="64" t="s">
@@ -7229,7 +7025,7 @@
     <row r="12" s="94" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="121" t="str">
         <f aca="false">Questionnaire!$A$23</f>
-        <v>2.1 Adherence to VGGT </v>
+        <v>2.1 Adherence to VGGT</v>
       </c>
       <c r="B12" s="122" t="str">
         <f aca="false">Questionnaire!J26</f>
@@ -7537,7 +7333,7 @@
     <row r="24" s="94" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="153" t="str">
         <f aca="false">Questionnaire!$A$68</f>
-        <v>4.1 Availability of food </v>
+        <v>4.1 Availability of food</v>
       </c>
       <c r="B24" s="122" t="n">
         <f aca="false">Questionnaire!J71</f>
@@ -7565,7 +7361,7 @@
     <row r="25" s="94" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="154" t="str">
         <f aca="false">Questionnaire!$A$72</f>
-        <v>4.2 Accessibility of food </v>
+        <v>4.2 Accessibility of food</v>
       </c>
       <c r="B25" s="126" t="n">
         <f aca="false">Questionnaire!J75</f>
@@ -7593,7 +7389,7 @@
     <row r="26" s="94" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="155" t="str">
         <f aca="false">Questionnaire!$A$76</f>
-        <v>4.3 Utilisation and nutritional adequacy </v>
+        <v>4.3 Utilisation and nutritional adequacy</v>
       </c>
       <c r="B26" s="126" t="n">
         <f aca="false">Questionnaire!J80</f>
@@ -7621,7 +7417,7 @@
     <row r="27" s="94" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="156" t="str">
         <f aca="false">Questionnaire!$A$81</f>
-        <v>4.4 Stability </v>
+        <v>4.4 Stability</v>
       </c>
       <c r="B27" s="129" t="n">
         <f aca="false">Questionnaire!J84</f>
@@ -8119,15 +7915,15 @@
       <selection pane="bottomLeft" activeCell="D114" activeCellId="0" sqref="D114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="207" width="30.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="208" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="56" width="7.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="56" width="1.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="56" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="56" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="56" width="1.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="56" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="56" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="56" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="65.86"/>
@@ -8144,7 +7940,7 @@
       </c>
       <c r="B1" s="210" t="str">
         <f aca="false">Profile!F1</f>
-        <v>Manga/ Lima</v>
+        <v>mango</v>
       </c>
       <c r="C1" s="64" t="s">
         <v>17</v>
@@ -11253,156 +11049,156 @@
     <mergeCell ref="A120:B120"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:H2">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
       <formula>"Substantial"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
       <formula>"Moderate"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
       <formula>"Substantial"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
       <formula>"Moderate"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
       <formula>"Substantial"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
       <formula>"Moderate"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
+    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="51">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26 A106 A92:K93 A107:K108 A118:B118 A119:J119 A113:J114 A109:J109 A99:J99 A94:J94 A73:J74 A62:K72 A95:K96 C106:K106 A110:K112 A115:K117 A120:K120 C26:K26 A3:K25 A27:K58 A75:K82 A84:K90 A83:E83 A100:K105">
-    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
+    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
+    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:E61">
-    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
+    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
+    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
+    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
+    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F59:K61">
-    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
+    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
+    <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
+    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
+    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="63">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91 C91:I91 K91">
-    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
+    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
+    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
+    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="66">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
+    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="67">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A97:K97 A98:J98">
-    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
+    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="68">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
+    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="69">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
+    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="70">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
+    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="71">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118:J118">
-    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
+    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="72">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="35" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
+    <cfRule type="cellIs" priority="35" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="73">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="36" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
+    <cfRule type="cellIs" priority="36" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="74">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
+    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="75">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J91">
-    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
+    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="76">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="39" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
+    <cfRule type="cellIs" priority="39" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="77">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="40" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
+    <cfRule type="cellIs" priority="40" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="78">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="41" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
+    <cfRule type="cellIs" priority="41" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="79">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F83:J83">
-    <cfRule type="cellIs" priority="42" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
+    <cfRule type="cellIs" priority="42" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="80">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
+    <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="81">
       <formula>$N$5</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="44" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110">
+    <cfRule type="cellIs" priority="44" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="82">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="45" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
+    <cfRule type="cellIs" priority="45" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="83">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11429,11 +11225,11 @@
   </sheetPr>
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="126"/>
@@ -11905,212 +11701,212 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <conditionalFormatting sqref="A25:B26 B40">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="84">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="85">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="86">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="87">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27">
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="88">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="89">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="90">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="91">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28">
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="92">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="93">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122">
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="94">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123">
+    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="95">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:B32">
-    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="96">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125">
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="97">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126">
+    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="98">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127">
+    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="99">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:B35">
-    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128">
+    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="100">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129">
+    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="101">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130">
+    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131">
+    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B33">
-    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132">
+    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133">
+    <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134">
+    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135">
+    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:B34">
-    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136">
+    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137">
+    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138">
+    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139">
+    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B36">
-    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140">
+    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141">
+    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142">
+    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143">
+    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B37">
-    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="144">
+    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="116">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="35" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="145">
+    <cfRule type="cellIs" priority="35" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="117">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="36" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="146">
+    <cfRule type="cellIs" priority="36" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="118">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="147">
+    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="119">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B38">
-    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="148">
+    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="120">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="39" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="149">
+    <cfRule type="cellIs" priority="39" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="121">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="40" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="150">
+    <cfRule type="cellIs" priority="40" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="122">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="41" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="151">
+    <cfRule type="cellIs" priority="41" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="123">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:B39">
-    <cfRule type="cellIs" priority="42" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="152">
+    <cfRule type="cellIs" priority="42" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="124">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="153">
+    <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="125">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="44" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="154">
+    <cfRule type="cellIs" priority="44" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="126">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="45" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="155">
+    <cfRule type="cellIs" priority="45" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="127">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44">
-    <cfRule type="cellIs" priority="46" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="156">
+    <cfRule type="cellIs" priority="46" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="128">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="47" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="157">
+    <cfRule type="cellIs" priority="47" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="129">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="48" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="158">
+    <cfRule type="cellIs" priority="48" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="130">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="159">
+    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="131">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="160">
+    <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="132">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="51" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="161">
+    <cfRule type="cellIs" priority="51" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="133">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="52" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="162">
+    <cfRule type="cellIs" priority="52" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="134">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="53" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="163">
+    <cfRule type="cellIs" priority="53" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="135">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45">
-    <cfRule type="cellIs" priority="54" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="164">
+    <cfRule type="cellIs" priority="54" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="136">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="55" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="165">
+    <cfRule type="cellIs" priority="55" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="137">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="56" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="166">
+    <cfRule type="cellIs" priority="56" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="138">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="57" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="167">
+    <cfRule type="cellIs" priority="57" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="139">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40">
-    <cfRule type="cellIs" priority="58" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="168">
+    <cfRule type="cellIs" priority="58" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="140">
       <formula>$N$6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="59" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="169">
+    <cfRule type="cellIs" priority="59" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="141">
       <formula>#ref!</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="60" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="170">
+    <cfRule type="cellIs" priority="60" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="142">
       <formula>$N$4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="61" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="171">
+    <cfRule type="cellIs" priority="61" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="143">
       <formula>$N$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>